<commit_message>
May Month code updated
</commit_message>
<xml_diff>
--- a/FastReact Confg..xlsx
+++ b/FastReact Confg..xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Capacity Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3696A50E-199F-4C60-AF2A-6A86E8A577F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAB6C5B-A442-4BE7-A72A-BF6761409BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9AFED8FC-535D-48D6-A46B-931961F691BE}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{9AFED8FC-535D-48D6-A46B-931961F691BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Report Name</t>
   </si>
@@ -135,10 +135,13 @@
     <t>Reports-Production-Unit Wise Plan Summary-All</t>
   </si>
   <si>
-    <t>Current Month</t>
-  </si>
-  <si>
     <t>Current Month+ 5</t>
+  </si>
+  <si>
+    <t>Unit wise Plan Qty</t>
+  </si>
+  <si>
+    <t>Reports-Planning-Buyer wise plan qty-Unit wise plan qty</t>
   </si>
 </sst>
 </file>
@@ -547,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293FE00B-EC13-46E8-B78F-2F1EC25697CE}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection sqref="A1:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,10 +591,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D2" s="7">
-        <v>45930</v>
+        <v>45961</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>7</v>
@@ -605,10 +608,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="7">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="D3" s="7">
-        <v>45930</v>
+        <v>45961</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>30</v>
@@ -622,13 +625,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="7">
-        <v>45748</v>
+        <v>45778</v>
       </c>
       <c r="D4" s="7">
-        <v>45930</v>
+        <v>45961</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -639,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D5" s="7">
-        <v>45930</v>
+        <v>45961</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>7</v>
@@ -656,10 +659,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D6" s="7">
-        <v>45930</v>
+        <v>45961</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
@@ -673,10 +676,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D7" s="7">
-        <v>45869</v>
+        <v>45900</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>18</v>
@@ -690,10 +693,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D8" s="7">
-        <v>45808</v>
+        <v>45838</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>21</v>
@@ -707,10 +710,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D9" s="7">
-        <v>45808</v>
+        <v>45838</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>21</v>
@@ -724,10 +727,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D10" s="7">
-        <v>45869</v>
+        <v>45900</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>18</v>
@@ -741,10 +744,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D11" s="7">
-        <v>45869</v>
+        <v>45900</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>18</v>
@@ -758,10 +761,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D12" s="7">
-        <v>45869</v>
+        <v>45900</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>18</v>
@@ -775,13 +778,30 @@
         <v>32</v>
       </c>
       <c r="C13" s="7">
-        <v>45748</v>
+        <v>45809</v>
       </c>
       <c r="D13" s="7">
-        <v>45777</v>
+        <v>45838</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>33</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="7">
+        <v>45809</v>
+      </c>
+      <c r="D14" s="7">
+        <v>45838</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
jun dates and blank days updated
</commit_message>
<xml_diff>
--- a/FastReact Confg..xlsx
+++ b/FastReact Confg..xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Capacity Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAB6C5B-A442-4BE7-A72A-BF6761409BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FF6ADE-E341-4081-BFE1-765039C7F57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{9AFED8FC-535D-48D6-A46B-931961F691BE}"/>
   </bookViews>
@@ -553,7 +553,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,10 +591,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D2" s="7">
-        <v>45961</v>
+        <v>45991</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>7</v>
@@ -608,10 +608,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D3" s="7">
-        <v>45961</v>
+        <v>45991</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>30</v>
@@ -625,10 +625,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="7">
-        <v>45778</v>
+        <v>45809</v>
       </c>
       <c r="D4" s="7">
-        <v>45961</v>
+        <v>45991</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>33</v>
@@ -642,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D5" s="7">
-        <v>45961</v>
+        <v>45991</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>7</v>
@@ -659,10 +659,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D6" s="7">
-        <v>45961</v>
+        <v>45991</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
@@ -676,10 +676,10 @@
         <v>17</v>
       </c>
       <c r="C7" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D7" s="7">
-        <v>45900</v>
+        <v>45930</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>18</v>
@@ -693,10 +693,10 @@
         <v>20</v>
       </c>
       <c r="C8" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D8" s="7">
-        <v>45838</v>
+        <v>45869</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>21</v>
@@ -710,10 +710,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D9" s="7">
-        <v>45838</v>
+        <v>45869</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>21</v>
@@ -727,10 +727,10 @@
         <v>24</v>
       </c>
       <c r="C10" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D10" s="7">
-        <v>45900</v>
+        <v>45930</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>18</v>
@@ -744,10 +744,10 @@
         <v>25</v>
       </c>
       <c r="C11" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D11" s="7">
-        <v>45900</v>
+        <v>45930</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>18</v>
@@ -761,10 +761,10 @@
         <v>27</v>
       </c>
       <c r="C12" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D12" s="7">
-        <v>45900</v>
+        <v>45930</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>18</v>
@@ -778,10 +778,10 @@
         <v>32</v>
       </c>
       <c r="C13" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D13" s="7">
-        <v>45838</v>
+        <v>45869</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>21</v>
@@ -795,10 +795,10 @@
         <v>35</v>
       </c>
       <c r="C14" s="7">
-        <v>45809</v>
+        <v>45839</v>
       </c>
       <c r="D14" s="7">
-        <v>45838</v>
+        <v>45869</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
feat(capacity_report): update script for February 2026 reporting
- Change file paths and month variables from December/January to February/March
- Adjust working days for February (22) and March (19) in capacity calculations
- Add logic to calculate and display factory-wise blank days percentage
- Reorganize final report layout: move titles, plan quantity, and add comparison section
- Remove outdated backup script file and old report PDFs
- Add new Excel templates for February reporting
</commit_message>
<xml_diff>
--- a/FastReact Confg..xlsx
+++ b/FastReact Confg..xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Work\1. Daily\Capacity Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA270FD3-543C-45FA-A47E-AB7FC03ED2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC51413C-8D5D-4C49-809B-204983A5B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{9AFED8FC-535D-48D6-A46B-931961F691BE}"/>
   </bookViews>
@@ -630,10 +630,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D3" s="8">
-        <v>46081</v>
+        <v>46234</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>7</v>
@@ -647,10 +647,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="8">
-        <v>45901</v>
+        <v>46054</v>
       </c>
       <c r="D4" s="8">
-        <v>46081</v>
+        <v>46234</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>30</v>
@@ -664,10 +664,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="8">
-        <v>45901</v>
+        <v>46054</v>
       </c>
       <c r="D5" s="8">
-        <v>46081</v>
+        <v>46234</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>33</v>
@@ -681,10 +681,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D6" s="8">
-        <v>46081</v>
+        <v>46234</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>7</v>
@@ -698,10 +698,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D7" s="8">
-        <v>46081</v>
+        <v>46234</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>7</v>
@@ -715,10 +715,10 @@
         <v>17</v>
       </c>
       <c r="C8" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D8" s="8">
-        <v>46022</v>
+        <v>46173</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>18</v>
@@ -732,10 +732,10 @@
         <v>20</v>
       </c>
       <c r="C9" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D9" s="8">
-        <v>45961</v>
+        <v>46112</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>21</v>
@@ -749,10 +749,10 @@
         <v>23</v>
       </c>
       <c r="C10" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D10" s="8">
-        <v>45961</v>
+        <v>46112</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>21</v>
@@ -766,10 +766,10 @@
         <v>24</v>
       </c>
       <c r="C11" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D11" s="8">
-        <v>46022</v>
+        <v>46173</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>18</v>
@@ -783,10 +783,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D12" s="8">
-        <v>46022</v>
+        <v>46173</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>18</v>
@@ -800,10 +800,10 @@
         <v>27</v>
       </c>
       <c r="C13" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D13" s="8">
-        <v>46022</v>
+        <v>46173</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>18</v>
@@ -817,10 +817,10 @@
         <v>32</v>
       </c>
       <c r="C14" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D14" s="8">
-        <v>45961</v>
+        <v>46112</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>21</v>
@@ -834,10 +834,10 @@
         <v>35</v>
       </c>
       <c r="C15" s="8">
-        <v>45931</v>
+        <v>46082</v>
       </c>
       <c r="D15" s="8">
-        <v>45961</v>
+        <v>46112</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>21</v>

</xml_diff>